<commit_message>
Add the perfect formula reducing several codes
</commit_message>
<xml_diff>
--- a/TA/Sample/rumus.xlsx
+++ b/TA/Sample/rumus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS_A455LD\Desktop\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wisely\Documents\GitHub\Thesis\TA\Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R78" sqref="R78"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P96" sqref="P96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>